<commit_message>
Completed Inventory Calculations for Cost
</commit_message>
<xml_diff>
--- a/testdata/sample mrp.xlsx
+++ b/testdata/sample mrp.xlsx
@@ -8,7 +8,7 @@
     <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId2"/>
+    <sheet name="Inventory" sheetId="1" state="visible" r:id="rId2"/>
     <sheet name="Sheet2" sheetId="2" state="visible" r:id="rId3"/>
     <sheet name="Sheet3" sheetId="3" state="visible" r:id="rId4"/>
   </sheets>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="189" uniqueCount="73">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="193" uniqueCount="76">
   <si>
     <t xml:space="preserve">PriceType</t>
   </si>
@@ -54,7 +54,7 @@
     <t xml:space="preserve">netcost</t>
   </si>
   <si>
-    <t xml:space="preserve">cost</t>
+    <t xml:space="preserve">cost1</t>
   </si>
   <si>
     <t xml:space="preserve">100</t>
@@ -78,7 +78,10 @@
     <t xml:space="preserve">47.29</t>
   </si>
   <si>
-    <t xml:space="preserve">0.5</t>
+    <t xml:space="preserve">0.50</t>
+  </si>
+  <si>
+    <t xml:space="preserve">cost2</t>
   </si>
   <si>
     <t xml:space="preserve">105</t>
@@ -102,7 +105,7 @@
     <t xml:space="preserve">48.21</t>
   </si>
   <si>
-    <t xml:space="preserve">0.50</t>
+    <t xml:space="preserve">cost3</t>
   </si>
   <si>
     <t xml:space="preserve">500.00</t>
@@ -114,6 +117,9 @@
     <t xml:space="preserve">448</t>
   </si>
   <si>
+    <t xml:space="preserve">cost4</t>
+  </si>
+  <si>
     <t xml:space="preserve">500</t>
   </si>
   <si>
@@ -124,6 +130,9 @@
   </si>
   <si>
     <t xml:space="preserve">436.58</t>
+  </si>
+  <si>
+    <t xml:space="preserve">cost5</t>
   </si>
   <si>
     <t xml:space="preserve">250</t>
@@ -251,7 +260,7 @@
     <numFmt numFmtId="164" formatCode="General"/>
     <numFmt numFmtId="165" formatCode="@"/>
   </numFmts>
-  <fonts count="7">
+  <fonts count="8">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -295,6 +304,12 @@
       <name val="Calibri"/>
       <family val="0"/>
       <charset val="134"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <name val="Arial"/>
+      <family val="0"/>
+      <charset val="1"/>
     </font>
   </fonts>
   <fills count="3">
@@ -359,7 +374,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -377,6 +392,10 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="165" fontId="6" fillId="2" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -399,18 +418,19 @@
   </sheetPr>
   <dimension ref="A1:J24"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E2" activeCellId="0" sqref="E2"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="F1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="N6" activeCellId="0" sqref="N6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.59765625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.640625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="1" style="1" width="9.14"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="1" style="1" width="9.13"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="24.83"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="27.85"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="1" width="24.86"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="1" width="24.87"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="1" width="19"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="1" width="10.58"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="8" style="1" width="18.14"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="8" style="1" width="18.12"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -445,7 +465,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="s">
         <v>10</v>
       </c>
@@ -477,41 +497,47 @@
         <v>47.05</v>
       </c>
     </row>
-    <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="5" t="s">
+        <v>19</v>
+      </c>
       <c r="B3" s="1" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="G3" s="1" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="H3" s="1" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="I3" s="1" t="s">
-        <v>26</v>
+        <v>18</v>
       </c>
       <c r="J3" s="0" t="n">
         <v>47.98</v>
       </c>
     </row>
-    <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="5" t="s">
+        <v>27</v>
+      </c>
       <c r="B4" s="1" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="D4" s="1" t="s">
         <v>16</v>
@@ -523,10 +549,10 @@
         <v>16</v>
       </c>
       <c r="G4" s="1" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="H4" s="1" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="I4" s="1" t="s">
         <v>16</v>
@@ -535,12 +561,15 @@
         <v>448</v>
       </c>
     </row>
-    <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="5" t="s">
+        <v>31</v>
+      </c>
       <c r="B5" s="1" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="D5" s="1" t="s">
         <v>16</v>
@@ -552,24 +581,27 @@
         <v>13</v>
       </c>
       <c r="G5" s="1" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="H5" s="1" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="I5" s="1" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="J5" s="0" t="n">
         <v>363.82</v>
       </c>
     </row>
-    <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="5" t="s">
+        <v>36</v>
+      </c>
       <c r="B6" s="1" t="s">
-        <v>34</v>
+        <v>37</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>35</v>
+        <v>38</v>
       </c>
       <c r="D6" s="1" t="s">
         <v>16</v>
@@ -581,10 +613,10 @@
         <v>16</v>
       </c>
       <c r="G6" s="1" t="s">
-        <v>36</v>
+        <v>39</v>
       </c>
       <c r="H6" s="1" t="s">
-        <v>37</v>
+        <v>40</v>
       </c>
       <c r="I6" s="1" t="s">
         <v>16</v>
@@ -604,10 +636,10 @@
         <v>2</v>
       </c>
       <c r="D7" s="3" t="s">
-        <v>38</v>
+        <v>41</v>
       </c>
       <c r="E7" s="3" t="s">
-        <v>39</v>
+        <v>42</v>
       </c>
       <c r="F7" s="3"/>
       <c r="G7" s="2" t="s">
@@ -623,15 +655,15 @@
         <v>9</v>
       </c>
     </row>
-    <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="1" t="s">
-        <v>40</v>
+        <v>43</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>41</v>
+        <v>44</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>42</v>
+        <v>45</v>
       </c>
       <c r="D8" s="1" t="s">
         <v>13</v>
@@ -643,7 +675,7 @@
         <v>16</v>
       </c>
       <c r="H8" s="1" t="s">
-        <v>43</v>
+        <v>46</v>
       </c>
       <c r="I8" s="1" t="s">
         <v>14</v>
@@ -654,10 +686,10 @@
     </row>
     <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B9" s="1" t="s">
-        <v>43</v>
+        <v>46</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>44</v>
+        <v>47</v>
       </c>
       <c r="D9" s="1" t="s">
         <v>16</v>
@@ -666,10 +698,10 @@
         <v>14</v>
       </c>
       <c r="G9" s="1" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="H9" s="1" t="s">
-        <v>43</v>
+        <v>46</v>
       </c>
       <c r="I9" s="1" t="s">
         <v>16</v>
@@ -680,22 +712,22 @@
     </row>
     <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B10" s="1" t="s">
-        <v>35</v>
+        <v>38</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>45</v>
+        <v>48</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="E10" s="1" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="G10" s="1" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="H10" s="1" t="s">
-        <v>46</v>
+        <v>49</v>
       </c>
       <c r="I10" s="1" t="s">
         <v>14</v>
@@ -706,10 +738,10 @@
     </row>
     <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B11" s="1" t="s">
-        <v>34</v>
+        <v>37</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>47</v>
+        <v>50</v>
       </c>
       <c r="D11" s="1" t="s">
         <v>16</v>
@@ -718,10 +750,10 @@
         <v>16</v>
       </c>
       <c r="G11" s="1" t="s">
-        <v>36</v>
+        <v>39</v>
       </c>
       <c r="H11" s="1" t="s">
-        <v>34</v>
+        <v>37</v>
       </c>
       <c r="I11" s="1" t="s">
         <v>16</v>
@@ -732,10 +764,10 @@
     </row>
     <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B12" s="1" t="s">
-        <v>48</v>
+        <v>51</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>49</v>
+        <v>52</v>
       </c>
       <c r="D12" s="1" t="s">
         <v>13</v>
@@ -744,10 +776,10 @@
         <v>16</v>
       </c>
       <c r="G12" s="1" t="s">
-        <v>50</v>
+        <v>53</v>
       </c>
       <c r="H12" s="1" t="s">
-        <v>48</v>
+        <v>51</v>
       </c>
       <c r="I12" s="1" t="s">
         <v>16</v>
@@ -767,10 +799,10 @@
         <v>2</v>
       </c>
       <c r="D13" s="3" t="s">
-        <v>38</v>
+        <v>41</v>
       </c>
       <c r="E13" s="3" t="s">
-        <v>39</v>
+        <v>42</v>
       </c>
       <c r="F13" s="3"/>
       <c r="G13" s="2" t="s">
@@ -788,28 +820,28 @@
     </row>
     <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="1" t="s">
-        <v>51</v>
+        <v>54</v>
       </c>
       <c r="B14" s="1" t="s">
         <v>11</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>52</v>
+        <v>55</v>
       </c>
       <c r="D14" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="E14" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="E14" s="1" t="s">
-        <v>21</v>
-      </c>
       <c r="G14" s="1" t="s">
         <v>16</v>
       </c>
       <c r="H14" s="1" t="s">
-        <v>53</v>
+        <v>56</v>
       </c>
       <c r="I14" s="1" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="J14" s="0" t="n">
         <v>72</v>
@@ -817,10 +849,10 @@
     </row>
     <row r="15" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B15" s="1" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>54</v>
+        <v>57</v>
       </c>
       <c r="D15" s="1" t="s">
         <v>14</v>
@@ -829,10 +861,10 @@
         <v>13</v>
       </c>
       <c r="G15" s="1" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="H15" s="1" t="s">
-        <v>55</v>
+        <v>58</v>
       </c>
       <c r="I15" s="1" t="s">
         <v>16</v>
@@ -843,10 +875,10 @@
     </row>
     <row r="16" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B16" s="1" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>56</v>
+        <v>59</v>
       </c>
       <c r="D16" s="1" t="s">
         <v>14</v>
@@ -855,10 +887,10 @@
         <v>13</v>
       </c>
       <c r="G16" s="1" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="H16" s="1" t="s">
-        <v>57</v>
+        <v>60</v>
       </c>
       <c r="I16" s="1" t="s">
         <v>16</v>
@@ -878,10 +910,10 @@
         <v>2</v>
       </c>
       <c r="D17" s="3" t="s">
-        <v>38</v>
+        <v>41</v>
       </c>
       <c r="E17" s="3" t="s">
-        <v>39</v>
+        <v>42</v>
       </c>
       <c r="F17" s="3"/>
       <c r="G17" s="2" t="s">
@@ -899,13 +931,13 @@
     </row>
     <row r="18" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="1" t="s">
-        <v>58</v>
+        <v>61</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>59</v>
+        <v>62</v>
       </c>
       <c r="D18" s="1" t="s">
         <v>13</v>
@@ -917,10 +949,10 @@
         <v>16</v>
       </c>
       <c r="H18" s="1" t="s">
-        <v>60</v>
+        <v>63</v>
       </c>
       <c r="I18" s="1" t="s">
-        <v>61</v>
+        <v>64</v>
       </c>
       <c r="J18" s="0" t="n">
         <v>9.8</v>
@@ -928,10 +960,10 @@
     </row>
     <row r="19" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B19" s="1" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>62</v>
+        <v>65</v>
       </c>
       <c r="D19" s="1" t="s">
         <v>13</v>
@@ -940,10 +972,10 @@
         <v>16</v>
       </c>
       <c r="G19" s="1" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="H19" s="1" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="I19" s="1" t="s">
         <v>16</v>
@@ -954,10 +986,10 @@
     </row>
     <row r="20" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B20" s="1" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>63</v>
+        <v>66</v>
       </c>
       <c r="D20" s="1" t="s">
         <v>14</v>
@@ -966,13 +998,13 @@
         <v>16</v>
       </c>
       <c r="G20" s="1" t="s">
-        <v>36</v>
+        <v>39</v>
       </c>
       <c r="H20" s="1" t="s">
-        <v>64</v>
+        <v>67</v>
       </c>
       <c r="I20" s="1" t="s">
-        <v>65</v>
+        <v>68</v>
       </c>
       <c r="J20" s="0" t="n">
         <v>34.7</v>
@@ -989,10 +1021,10 @@
         <v>2</v>
       </c>
       <c r="D21" s="3" t="s">
-        <v>38</v>
+        <v>41</v>
       </c>
       <c r="E21" s="3" t="s">
-        <v>39</v>
+        <v>42</v>
       </c>
       <c r="F21" s="3"/>
       <c r="G21" s="2" t="s">
@@ -1010,13 +1042,13 @@
     </row>
     <row r="22" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="1" t="s">
-        <v>66</v>
+        <v>69</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="C22" s="1" t="s">
-        <v>67</v>
+        <v>70</v>
       </c>
       <c r="D22" s="1" t="s">
         <v>13</v>
@@ -1028,7 +1060,7 @@
         <v>16</v>
       </c>
       <c r="H22" s="1" t="s">
-        <v>67</v>
+        <v>70</v>
       </c>
       <c r="I22" s="1" t="s">
         <v>16</v>
@@ -1039,10 +1071,10 @@
     </row>
     <row r="23" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B23" s="1" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="C23" s="1" t="s">
-        <v>68</v>
+        <v>71</v>
       </c>
       <c r="D23" s="1" t="s">
         <v>13</v>
@@ -1051,13 +1083,13 @@
         <v>14</v>
       </c>
       <c r="G23" s="1" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="H23" s="1" t="s">
-        <v>69</v>
+        <v>72</v>
       </c>
       <c r="I23" s="1" t="s">
-        <v>70</v>
+        <v>73</v>
       </c>
       <c r="J23" s="0" t="n">
         <v>20.38</v>
@@ -1065,10 +1097,10 @@
     </row>
     <row r="24" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B24" s="1" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="C24" s="1" t="s">
-        <v>63</v>
+        <v>66</v>
       </c>
       <c r="D24" s="1" t="s">
         <v>16</v>
@@ -1077,13 +1109,13 @@
         <v>14</v>
       </c>
       <c r="G24" s="1" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="H24" s="1" t="s">
-        <v>71</v>
+        <v>74</v>
       </c>
       <c r="I24" s="1" t="s">
-        <v>72</v>
+        <v>75</v>
       </c>
       <c r="J24" s="0" t="n">
         <v>32.92</v>
@@ -1111,7 +1143,7 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.59765625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.640625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData/>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
@@ -1134,7 +1166,7 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.59765625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.640625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData/>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>

</xml_diff>

<commit_message>
Added MRP Test Scenarios
</commit_message>
<xml_diff>
--- a/testdata/sample mrp.xlsx
+++ b/testdata/sample mrp.xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="193" uniqueCount="76">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="188" uniqueCount="77">
   <si>
     <t xml:space="preserve">PriceType</t>
   </si>
@@ -42,6 +42,12 @@
     <t xml:space="preserve">DiscountPer3</t>
   </si>
   <si>
+    <t xml:space="preserve">DiscountPer</t>
+  </si>
+  <si>
+    <t xml:space="preserve">AddDiscountPer</t>
+  </si>
+  <si>
     <t xml:space="preserve">GSTPer</t>
   </si>
   <si>
@@ -147,12 +153,6 @@
     <t xml:space="preserve">236</t>
   </si>
   <si>
-    <t xml:space="preserve">DiscountPer</t>
-  </si>
-  <si>
-    <t xml:space="preserve">AddDiscountPer</t>
-  </si>
-  <si>
     <t xml:space="preserve">MRP1</t>
   </si>
   <si>
@@ -244,6 +244,9 @@
   </si>
   <si>
     <t xml:space="preserve">3.90</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MRP5</t>
   </si>
   <si>
     <t xml:space="preserve">33.95</t>
@@ -401,39 +404,43 @@
     </xf>
   </cellXfs>
   <cellStyles count="6">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Comma" xfId="15" builtinId="3"/>
-    <cellStyle name="Comma [0]" xfId="16" builtinId="6"/>
-    <cellStyle name="Currency" xfId="17" builtinId="4"/>
-    <cellStyle name="Currency [0]" xfId="18" builtinId="7"/>
-    <cellStyle name="Percent" xfId="19" builtinId="5"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0" customBuiltin="false"/>
+    <cellStyle name="Comma" xfId="15" builtinId="3" customBuiltin="false"/>
+    <cellStyle name="Comma [0]" xfId="16" builtinId="6" customBuiltin="false"/>
+    <cellStyle name="Currency" xfId="17" builtinId="4" customBuiltin="false"/>
+    <cellStyle name="Currency [0]" xfId="18" builtinId="7" customBuiltin="false"/>
+    <cellStyle name="Percent" xfId="19" builtinId="5" customBuiltin="false"/>
   </cellStyles>
 </styleSheet>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:J24"/>
+  <dimension ref="A1:L24"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="F1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="N6" activeCellId="0" sqref="N6"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A12" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A24" activeCellId="0" sqref="A24"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.640625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="1" style="1" width="9.13"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="24.83"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="27.85"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="1" width="24.87"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="1" width="19"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="1" width="10.58"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="8" style="1" width="18.12"/>
+    <col collapsed="false" hidden="false" max="2" min="1" style="1" width="10.1224489795918"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="15.3877551020408"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="20.6530612244898"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="1" width="18.7295918367347"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="1" width="13.7704081632653"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="1" width="11.7448979591837"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="1" width="14.1020408163265"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="1" width="11.7448979591837"/>
+    <col collapsed="false" hidden="false" max="10" min="10" style="1" width="20.1479591836735"/>
+    <col collapsed="false" hidden="false" max="11" min="11" style="1" width="15.5969387755102"/>
+    <col collapsed="false" hidden="false" max="1025" min="12" style="0" width="9.62244897959184"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -452,180 +459,186 @@
       <c r="F1" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="2" t="s">
+      <c r="G1" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="2" t="s">
+      <c r="H1" s="3" t="s">
         <v>7</v>
       </c>
       <c r="I1" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="4" t="s">
+      <c r="J1" s="2" t="s">
         <v>9</v>
+      </c>
+      <c r="K1" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="L1" s="4" t="s">
+        <v>11</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="G2" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="H2" s="1" t="s">
         <v>17</v>
       </c>
       <c r="I2" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="J2" s="0" t="n">
+      <c r="J2" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="K2" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="L2" s="0" t="n">
         <v>47.05</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="5" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="B3" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="F3" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="I3" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="J3" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="K3" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="C3" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="D3" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="E3" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="F3" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="G3" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="H3" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="I3" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="J3" s="0" t="n">
+      <c r="L3" s="0" t="n">
         <v>47.98</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="E4" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="F4" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="I4" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="B4" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="C4" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="D4" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="E4" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="F4" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="G4" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="H4" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="I4" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="J4" s="0" t="n">
+      <c r="J4" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="K4" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="L4" s="0" t="n">
         <v>448</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="5" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="F5" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="G5" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="H5" s="1" t="s">
-        <v>35</v>
+        <v>15</v>
       </c>
       <c r="I5" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="J5" s="0" t="n">
+        <v>36</v>
+      </c>
+      <c r="J5" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="K5" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="L5" s="0" t="n">
         <v>363.82</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="5" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="F6" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="G6" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="H6" s="1" t="s">
-        <v>40</v>
+        <v>18</v>
       </c>
       <c r="I6" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="J6" s="0" t="n">
+        <v>41</v>
+      </c>
+      <c r="J6" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="K6" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="L6" s="0" t="n">
         <v>236</v>
       </c>
     </row>
-    <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="2" t="s">
         <v>0</v>
       </c>
@@ -635,24 +648,22 @@
       <c r="C7" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D7" s="3" t="s">
-        <v>41</v>
-      </c>
-      <c r="E7" s="3" t="s">
-        <v>42</v>
-      </c>
+      <c r="D7" s="3"/>
+      <c r="E7" s="3"/>
       <c r="F7" s="3"/>
-      <c r="G7" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="H7" s="2" t="s">
-        <v>7</v>
-      </c>
+      <c r="G7" s="3"/>
+      <c r="H7" s="3"/>
       <c r="I7" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="J7" s="4" t="s">
+      <c r="J7" s="2" t="s">
         <v>9</v>
+      </c>
+      <c r="K7" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="L7" s="4" t="s">
+        <v>11</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -665,130 +676,130 @@
       <c r="C8" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="D8" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="E8" s="1" t="s">
-        <v>14</v>
-      </c>
       <c r="G8" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="H8" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="H8" s="1" t="s">
+      <c r="I8" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="J8" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="I8" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="J8" s="0" t="n">
+      <c r="K8" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="L8" s="0" t="n">
         <v>97.02</v>
       </c>
     </row>
-    <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B9" s="1" t="s">
         <v>46</v>
       </c>
       <c r="C9" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="D9" s="1" t="s">
+      <c r="G9" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="H9" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="E9" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="G9" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="H9" s="1" t="s">
+      <c r="I9" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="J9" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="I9" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="J9" s="0" t="n">
+      <c r="K9" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="L9" s="0" t="n">
         <v>96.04</v>
       </c>
     </row>
-    <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B10" s="1" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="C10" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="D10" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="E10" s="1" t="s">
-        <v>23</v>
-      </c>
       <c r="G10" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="H10" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="H10" s="1" t="s">
+      <c r="I10" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="J10" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="I10" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="J10" s="0" t="n">
+      <c r="K10" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="L10" s="0" t="n">
         <v>144</v>
       </c>
     </row>
-    <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B11" s="1" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="C11" s="1" t="s">
         <v>50</v>
       </c>
-      <c r="D11" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="E11" s="1" t="s">
-        <v>16</v>
-      </c>
       <c r="G11" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="H11" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="I11" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="J11" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="H11" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="I11" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="J11" s="0" t="n">
+      <c r="K11" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="L11" s="0" t="n">
         <v>250</v>
       </c>
     </row>
-    <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B12" s="1" t="s">
         <v>51</v>
       </c>
       <c r="C12" s="1" t="s">
         <v>52</v>
       </c>
-      <c r="D12" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="E12" s="1" t="s">
-        <v>16</v>
-      </c>
       <c r="G12" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="H12" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="I12" s="1" t="s">
         <v>53</v>
       </c>
-      <c r="H12" s="1" t="s">
+      <c r="J12" s="1" t="s">
         <v>51</v>
       </c>
-      <c r="I12" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="J12" s="0" t="n">
+      <c r="K12" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="L12" s="0" t="n">
         <v>148.5</v>
       </c>
     </row>
-    <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="2" t="s">
         <v>0</v>
       </c>
@@ -798,108 +809,106 @@
       <c r="C13" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D13" s="3" t="s">
-        <v>41</v>
-      </c>
-      <c r="E13" s="3" t="s">
-        <v>42</v>
-      </c>
+      <c r="D13" s="3"/>
+      <c r="E13" s="3"/>
       <c r="F13" s="3"/>
-      <c r="G13" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="H13" s="2" t="s">
-        <v>7</v>
-      </c>
+      <c r="G13" s="3"/>
+      <c r="H13" s="3"/>
       <c r="I13" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="J13" s="4" t="s">
+      <c r="J13" s="2" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="K13" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="L13" s="4" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="1" t="s">
         <v>54</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="C14" s="1" t="s">
         <v>55</v>
       </c>
-      <c r="D14" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="E14" s="1" t="s">
-        <v>22</v>
-      </c>
       <c r="G14" s="1" t="s">
-        <v>16</v>
+        <v>25</v>
       </c>
       <c r="H14" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="I14" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="J14" s="1" t="s">
         <v>56</v>
       </c>
-      <c r="I14" s="1" t="s">
+      <c r="K14" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="L14" s="0" t="n">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B15" s="1" t="s">
         <v>34</v>
-      </c>
-      <c r="J14" s="0" t="n">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="15" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B15" s="1" t="s">
-        <v>32</v>
       </c>
       <c r="C15" s="1" t="s">
         <v>57</v>
       </c>
-      <c r="D15" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="E15" s="1" t="s">
-        <v>13</v>
-      </c>
       <c r="G15" s="1" t="s">
-        <v>34</v>
+        <v>16</v>
       </c>
       <c r="H15" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="I15" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="J15" s="1" t="s">
         <v>58</v>
       </c>
-      <c r="I15" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="J15" s="0" t="n">
+      <c r="K15" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="L15" s="0" t="n">
         <v>485.1</v>
       </c>
     </row>
-    <row r="16" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B16" s="1" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="C16" s="1" t="s">
         <v>59</v>
       </c>
-      <c r="D16" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="E16" s="1" t="s">
-        <v>13</v>
-      </c>
       <c r="G16" s="1" t="s">
-        <v>25</v>
+        <v>16</v>
       </c>
       <c r="H16" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="I16" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="J16" s="1" t="s">
         <v>60</v>
       </c>
-      <c r="I16" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="J16" s="0" t="n">
+      <c r="K16" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="L16" s="0" t="n">
         <v>9.7</v>
       </c>
     </row>
-    <row r="17" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="2" t="s">
         <v>0</v>
       </c>
@@ -909,108 +918,106 @@
       <c r="C17" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D17" s="3" t="s">
-        <v>41</v>
-      </c>
-      <c r="E17" s="3" t="s">
-        <v>42</v>
-      </c>
+      <c r="D17" s="3"/>
+      <c r="E17" s="3"/>
       <c r="F17" s="3"/>
-      <c r="G17" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="H17" s="2" t="s">
-        <v>7</v>
-      </c>
+      <c r="G17" s="3"/>
+      <c r="H17" s="3"/>
       <c r="I17" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="J17" s="4" t="s">
+      <c r="J17" s="2" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="18" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="K17" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="L17" s="4" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="18" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="1" t="s">
         <v>61</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="C18" s="1" t="s">
         <v>62</v>
       </c>
-      <c r="D18" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="E18" s="1" t="s">
-        <v>13</v>
-      </c>
       <c r="G18" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="H18" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="I18" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="J18" s="1" t="s">
         <v>63</v>
       </c>
-      <c r="I18" s="1" t="s">
+      <c r="K18" s="1" t="s">
         <v>64</v>
       </c>
-      <c r="J18" s="0" t="n">
+      <c r="L18" s="0" t="n">
         <v>9.8</v>
       </c>
     </row>
-    <row r="19" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="19" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B19" s="1" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="C19" s="1" t="s">
         <v>65</v>
       </c>
-      <c r="D19" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="E19" s="1" t="s">
-        <v>16</v>
-      </c>
       <c r="G19" s="1" t="s">
-        <v>34</v>
+        <v>15</v>
       </c>
       <c r="H19" s="1" t="s">
-        <v>23</v>
+        <v>18</v>
       </c>
       <c r="I19" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="J19" s="0" t="n">
+        <v>36</v>
+      </c>
+      <c r="J19" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="K19" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="L19" s="0" t="n">
         <v>20.78</v>
       </c>
     </row>
-    <row r="20" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="20" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B20" s="1" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="C20" s="1" t="s">
         <v>66</v>
       </c>
-      <c r="D20" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="E20" s="1" t="s">
+      <c r="G20" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="G20" s="1" t="s">
-        <v>39</v>
-      </c>
       <c r="H20" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="I20" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="J20" s="1" t="s">
         <v>67</v>
       </c>
-      <c r="I20" s="1" t="s">
+      <c r="K20" s="1" t="s">
         <v>68</v>
       </c>
-      <c r="J20" s="0" t="n">
+      <c r="L20" s="0" t="n">
         <v>34.7</v>
       </c>
     </row>
-    <row r="21" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="21" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="2" t="s">
         <v>0</v>
       </c>
@@ -1020,111 +1027,112 @@
       <c r="C21" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D21" s="3" t="s">
-        <v>41</v>
-      </c>
-      <c r="E21" s="3" t="s">
-        <v>42</v>
-      </c>
+      <c r="D21" s="3"/>
+      <c r="E21" s="3"/>
       <c r="F21" s="3"/>
-      <c r="G21" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="H21" s="2" t="s">
-        <v>7</v>
-      </c>
+      <c r="G21" s="3"/>
+      <c r="H21" s="3"/>
       <c r="I21" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="J21" s="4" t="s">
+      <c r="J21" s="2" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="22" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="K21" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="L21" s="4" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="22" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="1" t="s">
         <v>69</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="C22" s="1" t="s">
         <v>70</v>
       </c>
-      <c r="D22" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="E22" s="1" t="s">
-        <v>14</v>
-      </c>
       <c r="G22" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="H22" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="H22" s="1" t="s">
+      <c r="I22" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="J22" s="1" t="s">
         <v>70</v>
       </c>
-      <c r="I22" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="J22" s="0" t="n">
+      <c r="K22" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="L22" s="0" t="n">
         <v>9.7</v>
       </c>
     </row>
-    <row r="23" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="23" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B23" s="1" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="C23" s="1" t="s">
         <v>71</v>
       </c>
-      <c r="D23" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="E23" s="1" t="s">
-        <v>14</v>
-      </c>
       <c r="G23" s="1" t="s">
-        <v>34</v>
+        <v>15</v>
       </c>
       <c r="H23" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="I23" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="J23" s="1" t="s">
         <v>72</v>
       </c>
-      <c r="I23" s="1" t="s">
+      <c r="K23" s="1" t="s">
         <v>73</v>
       </c>
-      <c r="J23" s="0" t="n">
+      <c r="L23" s="0" t="n">
         <v>20.38</v>
       </c>
     </row>
-    <row r="24" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="24" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A24" s="1" t="s">
+        <v>74</v>
+      </c>
       <c r="B24" s="1" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="C24" s="1" t="s">
         <v>66</v>
       </c>
-      <c r="D24" s="1" t="s">
+      <c r="G24" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="H24" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="E24" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="G24" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="H24" s="1" t="s">
-        <v>74</v>
-      </c>
       <c r="I24" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="J24" s="1" t="s">
         <v>75</v>
       </c>
-      <c r="J24" s="0" t="n">
+      <c r="K24" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="L24" s="0" t="n">
         <v>32.92</v>
       </c>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader/>
     <oddFooter/>
@@ -1133,7 +1141,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
@@ -1143,11 +1151,14 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.640625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="9.62244897959184"/>
+  </cols>
   <sheetData/>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader/>
     <oddFooter/>
@@ -1156,7 +1167,7 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
@@ -1166,11 +1177,14 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.640625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="9.62244897959184"/>
+  </cols>
   <sheetData/>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader/>
     <oddFooter/>

</xml_diff>

<commit_message>
new inventory data from excel sheet
committed. (new inventory + calculation from excel sheet)
</commit_message>
<xml_diff>
--- a/testdata/sample mrp.xlsx
+++ b/testdata/sample mrp.xlsx
@@ -9,8 +9,7 @@
   </bookViews>
   <sheets>
     <sheet name="Inventory" sheetId="1" state="visible" r:id="rId2"/>
-    <sheet name="Sheet2" sheetId="2" state="visible" r:id="rId3"/>
-    <sheet name="Sheet3" sheetId="3" state="visible" r:id="rId4"/>
+    <sheet name="Sheet3" sheetId="2" state="visible" r:id="rId3"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
   <extLst>
@@ -22,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="188" uniqueCount="77">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="208" uniqueCount="97">
   <si>
     <t xml:space="preserve">PriceType</t>
   </si>
@@ -60,6 +59,42 @@
     <t xml:space="preserve">netcost</t>
   </si>
   <si>
+    <t xml:space="preserve">InventoryType</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Category</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Department</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Brand</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Item Name</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Short Name</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Item Type</t>
+  </si>
+  <si>
+    <t xml:space="preserve">UOM Purchase</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Sales UOM</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Stock Type</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Vendor</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Floor</t>
+  </si>
+  <si>
     <t xml:space="preserve">cost1</t>
   </si>
   <si>
@@ -85,6 +120,30 @@
   </si>
   <si>
     <t xml:space="preserve">0.50</t>
+  </si>
+  <si>
+    <t xml:space="preserve">inventory</t>
+  </si>
+  <si>
+    <t xml:space="preserve">BISCUITS</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SNACKS</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PARLE</t>
+  </si>
+  <si>
+    <t xml:space="preserve">BISC Test Parle</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PARLEs</t>
+  </si>
+  <si>
+    <t xml:space="preserve">BULK</t>
+  </si>
+  <si>
+    <t xml:space="preserve">AKSHAYA TRADERS</t>
   </si>
   <si>
     <t xml:space="preserve">cost2</t>
@@ -419,25 +478,25 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:L24"/>
+  <dimension ref="A1:X24"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A12" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A24" activeCellId="0" sqref="A24"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="L1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="S2" activeCellId="0" sqref="S2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="2" min="1" style="1" width="10.1224489795918"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="15.3877551020408"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="20.6530612244898"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="1" width="18.7295918367347"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="1" width="13.7704081632653"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="1" width="11.7448979591837"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="1" width="14.1020408163265"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="1" width="11.7448979591837"/>
-    <col collapsed="false" hidden="false" max="10" min="10" style="1" width="20.1479591836735"/>
-    <col collapsed="false" hidden="false" max="11" min="11" style="1" width="15.5969387755102"/>
-    <col collapsed="false" hidden="false" max="1025" min="12" style="0" width="9.62244897959184"/>
+    <col collapsed="false" hidden="false" max="2" min="1" style="1" width="13.0561224489796"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="20.3469387755102"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="27.3418367346939"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="1" width="24.7040816326531"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="1" width="18.2244897959184"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="1" width="15.4897959183673"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="1" width="18.6275510204082"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="1" width="15.4897959183673"/>
+    <col collapsed="false" hidden="false" max="10" min="10" style="1" width="26.7295918367347"/>
+    <col collapsed="false" hidden="false" max="11" min="11" style="1" width="20.5561224489796"/>
+    <col collapsed="false" hidden="false" max="1025" min="12" style="0" width="12.3571428571429"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -477,66 +536,126 @@
       <c r="L1" s="4" t="s">
         <v>11</v>
       </c>
+      <c r="M1" s="0" t="s">
+        <v>12</v>
+      </c>
+      <c r="N1" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="O1" s="0" t="s">
+        <v>14</v>
+      </c>
+      <c r="P1" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="Q1" s="0" t="s">
+        <v>16</v>
+      </c>
+      <c r="R1" s="0" t="s">
+        <v>17</v>
+      </c>
+      <c r="S1" s="0" t="s">
+        <v>18</v>
+      </c>
+      <c r="T1" s="0" t="s">
+        <v>19</v>
+      </c>
+      <c r="U1" s="0" t="s">
+        <v>20</v>
+      </c>
+      <c r="V1" s="0" t="s">
+        <v>21</v>
+      </c>
+      <c r="W1" s="0" t="s">
+        <v>22</v>
+      </c>
+      <c r="X1" s="0" t="s">
+        <v>23</v>
+      </c>
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="s">
-        <v>12</v>
+        <v>24</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>13</v>
+        <v>25</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>14</v>
+        <v>26</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>15</v>
+        <v>27</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>16</v>
+        <v>28</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>17</v>
+        <v>29</v>
       </c>
       <c r="I2" s="1" t="s">
-        <v>18</v>
+        <v>30</v>
       </c>
       <c r="J2" s="1" t="s">
-        <v>19</v>
+        <v>31</v>
       </c>
       <c r="K2" s="1" t="s">
-        <v>20</v>
+        <v>32</v>
       </c>
       <c r="L2" s="0" t="n">
         <v>47.05</v>
       </c>
+      <c r="M2" s="0" t="s">
+        <v>33</v>
+      </c>
+      <c r="N2" s="0" t="s">
+        <v>34</v>
+      </c>
+      <c r="O2" s="0" t="s">
+        <v>35</v>
+      </c>
+      <c r="P2" s="0" t="s">
+        <v>36</v>
+      </c>
+      <c r="Q2" s="0" t="s">
+        <v>37</v>
+      </c>
+      <c r="R2" s="0" t="s">
+        <v>38</v>
+      </c>
+      <c r="S2" s="0" t="s">
+        <v>39</v>
+      </c>
+      <c r="W2" s="0" t="s">
+        <v>40</v>
+      </c>
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="5" t="s">
-        <v>21</v>
+        <v>41</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>22</v>
+        <v>42</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>23</v>
+        <v>43</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>24</v>
+        <v>44</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>25</v>
+        <v>45</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>26</v>
+        <v>46</v>
       </c>
       <c r="I3" s="1" t="s">
-        <v>27</v>
+        <v>47</v>
       </c>
       <c r="J3" s="1" t="s">
-        <v>28</v>
+        <v>48</v>
       </c>
       <c r="K3" s="1" t="s">
-        <v>20</v>
+        <v>32</v>
       </c>
       <c r="L3" s="0" t="n">
         <v>47.98</v>
@@ -544,31 +663,31 @@
     </row>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="5" t="s">
-        <v>29</v>
+        <v>49</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>30</v>
+        <v>50</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>31</v>
+        <v>51</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>18</v>
+        <v>30</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>18</v>
+        <v>30</v>
       </c>
       <c r="F4" s="1" t="s">
-        <v>18</v>
+        <v>30</v>
       </c>
       <c r="I4" s="1" t="s">
-        <v>27</v>
+        <v>47</v>
       </c>
       <c r="J4" s="1" t="s">
-        <v>32</v>
+        <v>52</v>
       </c>
       <c r="K4" s="1" t="s">
-        <v>18</v>
+        <v>30</v>
       </c>
       <c r="L4" s="0" t="n">
         <v>448</v>
@@ -576,31 +695,31 @@
     </row>
     <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="5" t="s">
-        <v>33</v>
+        <v>53</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>34</v>
+        <v>54</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>35</v>
+        <v>55</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>18</v>
+        <v>30</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>18</v>
+        <v>30</v>
       </c>
       <c r="F5" s="1" t="s">
-        <v>15</v>
+        <v>27</v>
       </c>
       <c r="I5" s="1" t="s">
-        <v>36</v>
+        <v>56</v>
       </c>
       <c r="J5" s="1" t="s">
-        <v>37</v>
+        <v>57</v>
       </c>
       <c r="K5" s="1" t="s">
-        <v>25</v>
+        <v>45</v>
       </c>
       <c r="L5" s="0" t="n">
         <v>363.82</v>
@@ -608,31 +727,31 @@
     </row>
     <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="5" t="s">
-        <v>38</v>
+        <v>58</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>39</v>
+        <v>59</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>40</v>
+        <v>60</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>18</v>
+        <v>30</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>18</v>
+        <v>30</v>
       </c>
       <c r="F6" s="1" t="s">
-        <v>18</v>
+        <v>30</v>
       </c>
       <c r="I6" s="1" t="s">
-        <v>41</v>
+        <v>61</v>
       </c>
       <c r="J6" s="1" t="s">
-        <v>42</v>
+        <v>62</v>
       </c>
       <c r="K6" s="1" t="s">
-        <v>18</v>
+        <v>30</v>
       </c>
       <c r="L6" s="0" t="n">
         <v>236</v>
@@ -668,28 +787,28 @@
     </row>
     <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="1" t="s">
-        <v>43</v>
+        <v>63</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>44</v>
+        <v>64</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>45</v>
+        <v>65</v>
       </c>
       <c r="G8" s="1" t="s">
-        <v>15</v>
+        <v>27</v>
       </c>
       <c r="H8" s="1" t="s">
-        <v>16</v>
+        <v>28</v>
       </c>
       <c r="I8" s="1" t="s">
-        <v>18</v>
+        <v>30</v>
       </c>
       <c r="J8" s="1" t="s">
-        <v>46</v>
+        <v>66</v>
       </c>
       <c r="K8" s="1" t="s">
-        <v>16</v>
+        <v>28</v>
       </c>
       <c r="L8" s="0" t="n">
         <v>97.02</v>
@@ -697,25 +816,25 @@
     </row>
     <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B9" s="1" t="s">
-        <v>46</v>
+        <v>66</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>47</v>
+        <v>67</v>
       </c>
       <c r="G9" s="1" t="s">
-        <v>18</v>
+        <v>30</v>
       </c>
       <c r="H9" s="1" t="s">
-        <v>16</v>
+        <v>28</v>
       </c>
       <c r="I9" s="1" t="s">
-        <v>36</v>
+        <v>56</v>
       </c>
       <c r="J9" s="1" t="s">
-        <v>46</v>
+        <v>66</v>
       </c>
       <c r="K9" s="1" t="s">
-        <v>18</v>
+        <v>30</v>
       </c>
       <c r="L9" s="0" t="n">
         <v>96.04</v>
@@ -723,25 +842,25 @@
     </row>
     <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B10" s="1" t="s">
-        <v>40</v>
+        <v>60</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>48</v>
+        <v>68</v>
       </c>
       <c r="G10" s="1" t="s">
-        <v>24</v>
+        <v>44</v>
       </c>
       <c r="H10" s="1" t="s">
-        <v>25</v>
+        <v>45</v>
       </c>
       <c r="I10" s="1" t="s">
-        <v>27</v>
+        <v>47</v>
       </c>
       <c r="J10" s="1" t="s">
-        <v>49</v>
+        <v>69</v>
       </c>
       <c r="K10" s="1" t="s">
-        <v>16</v>
+        <v>28</v>
       </c>
       <c r="L10" s="0" t="n">
         <v>144</v>
@@ -749,25 +868,25 @@
     </row>
     <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B11" s="1" t="s">
-        <v>39</v>
+        <v>59</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>50</v>
+        <v>70</v>
       </c>
       <c r="G11" s="1" t="s">
-        <v>18</v>
+        <v>30</v>
       </c>
       <c r="H11" s="1" t="s">
-        <v>18</v>
+        <v>30</v>
       </c>
       <c r="I11" s="1" t="s">
-        <v>41</v>
+        <v>61</v>
       </c>
       <c r="J11" s="1" t="s">
-        <v>39</v>
+        <v>59</v>
       </c>
       <c r="K11" s="1" t="s">
-        <v>18</v>
+        <v>30</v>
       </c>
       <c r="L11" s="0" t="n">
         <v>250</v>
@@ -775,25 +894,25 @@
     </row>
     <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B12" s="1" t="s">
-        <v>51</v>
+        <v>71</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>52</v>
+        <v>72</v>
       </c>
       <c r="G12" s="1" t="s">
-        <v>15</v>
+        <v>27</v>
       </c>
       <c r="H12" s="1" t="s">
-        <v>18</v>
+        <v>30</v>
       </c>
       <c r="I12" s="1" t="s">
-        <v>53</v>
+        <v>73</v>
       </c>
       <c r="J12" s="1" t="s">
-        <v>51</v>
+        <v>71</v>
       </c>
       <c r="K12" s="1" t="s">
-        <v>18</v>
+        <v>30</v>
       </c>
       <c r="L12" s="0" t="n">
         <v>148.5</v>
@@ -829,28 +948,28 @@
     </row>
     <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="1" t="s">
-        <v>54</v>
+        <v>74</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>13</v>
+        <v>25</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>55</v>
+        <v>75</v>
       </c>
       <c r="G14" s="1" t="s">
-        <v>25</v>
+        <v>45</v>
       </c>
       <c r="H14" s="1" t="s">
-        <v>24</v>
+        <v>44</v>
       </c>
       <c r="I14" s="1" t="s">
-        <v>18</v>
+        <v>30</v>
       </c>
       <c r="J14" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="K14" s="1" t="s">
         <v>56</v>
-      </c>
-      <c r="K14" s="1" t="s">
-        <v>36</v>
       </c>
       <c r="L14" s="0" t="n">
         <v>72</v>
@@ -858,25 +977,25 @@
     </row>
     <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B15" s="1" t="s">
-        <v>34</v>
+        <v>54</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>57</v>
+        <v>77</v>
       </c>
       <c r="G15" s="1" t="s">
-        <v>16</v>
+        <v>28</v>
       </c>
       <c r="H15" s="1" t="s">
-        <v>15</v>
+        <v>27</v>
       </c>
       <c r="I15" s="1" t="s">
-        <v>36</v>
+        <v>56</v>
       </c>
       <c r="J15" s="1" t="s">
-        <v>58</v>
+        <v>78</v>
       </c>
       <c r="K15" s="1" t="s">
-        <v>18</v>
+        <v>30</v>
       </c>
       <c r="L15" s="0" t="n">
         <v>485.1</v>
@@ -884,25 +1003,25 @@
     </row>
     <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B16" s="1" t="s">
-        <v>24</v>
+        <v>44</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>59</v>
+        <v>79</v>
       </c>
       <c r="G16" s="1" t="s">
-        <v>16</v>
+        <v>28</v>
       </c>
       <c r="H16" s="1" t="s">
-        <v>15</v>
+        <v>27</v>
       </c>
       <c r="I16" s="1" t="s">
-        <v>27</v>
+        <v>47</v>
       </c>
       <c r="J16" s="1" t="s">
-        <v>60</v>
+        <v>80</v>
       </c>
       <c r="K16" s="1" t="s">
-        <v>18</v>
+        <v>30</v>
       </c>
       <c r="L16" s="0" t="n">
         <v>9.7</v>
@@ -938,28 +1057,28 @@
     </row>
     <row r="18" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="1" t="s">
-        <v>61</v>
+        <v>81</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>24</v>
+        <v>44</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>62</v>
+        <v>82</v>
       </c>
       <c r="G18" s="1" t="s">
-        <v>15</v>
+        <v>27</v>
       </c>
       <c r="H18" s="1" t="s">
-        <v>15</v>
+        <v>27</v>
       </c>
       <c r="I18" s="1" t="s">
-        <v>18</v>
+        <v>30</v>
       </c>
       <c r="J18" s="1" t="s">
-        <v>63</v>
+        <v>83</v>
       </c>
       <c r="K18" s="1" t="s">
-        <v>64</v>
+        <v>84</v>
       </c>
       <c r="L18" s="0" t="n">
         <v>9.8</v>
@@ -967,25 +1086,25 @@
     </row>
     <row r="19" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B19" s="1" t="s">
-        <v>25</v>
+        <v>45</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>65</v>
+        <v>85</v>
       </c>
       <c r="G19" s="1" t="s">
-        <v>15</v>
+        <v>27</v>
       </c>
       <c r="H19" s="1" t="s">
-        <v>18</v>
+        <v>30</v>
       </c>
       <c r="I19" s="1" t="s">
-        <v>36</v>
+        <v>56</v>
       </c>
       <c r="J19" s="1" t="s">
-        <v>25</v>
+        <v>45</v>
       </c>
       <c r="K19" s="1" t="s">
-        <v>18</v>
+        <v>30</v>
       </c>
       <c r="L19" s="0" t="n">
         <v>20.78</v>
@@ -993,25 +1112,25 @@
     </row>
     <row r="20" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B20" s="1" t="s">
-        <v>26</v>
+        <v>46</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>66</v>
+        <v>86</v>
       </c>
       <c r="G20" s="1" t="s">
-        <v>16</v>
+        <v>28</v>
       </c>
       <c r="H20" s="1" t="s">
-        <v>18</v>
+        <v>30</v>
       </c>
       <c r="I20" s="1" t="s">
-        <v>41</v>
+        <v>61</v>
       </c>
       <c r="J20" s="1" t="s">
-        <v>67</v>
+        <v>87</v>
       </c>
       <c r="K20" s="1" t="s">
-        <v>68</v>
+        <v>88</v>
       </c>
       <c r="L20" s="0" t="n">
         <v>34.7</v>
@@ -1047,28 +1166,28 @@
     </row>
     <row r="22" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="1" t="s">
-        <v>69</v>
+        <v>89</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>24</v>
+        <v>44</v>
       </c>
       <c r="C22" s="1" t="s">
-        <v>70</v>
+        <v>90</v>
       </c>
       <c r="G22" s="1" t="s">
-        <v>15</v>
+        <v>27</v>
       </c>
       <c r="H22" s="1" t="s">
-        <v>16</v>
+        <v>28</v>
       </c>
       <c r="I22" s="1" t="s">
-        <v>18</v>
+        <v>30</v>
       </c>
       <c r="J22" s="1" t="s">
-        <v>70</v>
+        <v>90</v>
       </c>
       <c r="K22" s="1" t="s">
-        <v>18</v>
+        <v>30</v>
       </c>
       <c r="L22" s="0" t="n">
         <v>9.7</v>
@@ -1076,25 +1195,25 @@
     </row>
     <row r="23" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B23" s="1" t="s">
-        <v>25</v>
+        <v>45</v>
       </c>
       <c r="C23" s="1" t="s">
-        <v>71</v>
+        <v>91</v>
       </c>
       <c r="G23" s="1" t="s">
-        <v>15</v>
+        <v>27</v>
       </c>
       <c r="H23" s="1" t="s">
-        <v>16</v>
+        <v>28</v>
       </c>
       <c r="I23" s="1" t="s">
-        <v>36</v>
+        <v>56</v>
       </c>
       <c r="J23" s="1" t="s">
-        <v>72</v>
+        <v>92</v>
       </c>
       <c r="K23" s="1" t="s">
-        <v>73</v>
+        <v>93</v>
       </c>
       <c r="L23" s="0" t="n">
         <v>20.38</v>
@@ -1102,28 +1221,28 @@
     </row>
     <row r="24" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="1" t="s">
-        <v>74</v>
+        <v>94</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>26</v>
+        <v>46</v>
       </c>
       <c r="C24" s="1" t="s">
-        <v>66</v>
+        <v>86</v>
       </c>
       <c r="G24" s="1" t="s">
-        <v>18</v>
+        <v>30</v>
       </c>
       <c r="H24" s="1" t="s">
-        <v>16</v>
+        <v>28</v>
       </c>
       <c r="I24" s="1" t="s">
-        <v>27</v>
+        <v>47</v>
       </c>
       <c r="J24" s="1" t="s">
-        <v>75</v>
+        <v>95</v>
       </c>
       <c r="K24" s="1" t="s">
-        <v>76</v>
+        <v>96</v>
       </c>
       <c r="L24" s="0" t="n">
         <v>32.92</v>
@@ -1153,33 +1272,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="9.62244897959184"/>
-  </cols>
-  <sheetData/>
-  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
-  <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader/>
-    <oddFooter/>
-  </headerFooter>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <sheetPr filterMode="false">
-    <pageSetUpPr fitToPage="false"/>
-  </sheetPr>
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
-  <cols>
-    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="9.62244897959184"/>
+    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="12.3571428571429"/>
   </cols>
   <sheetData/>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>

</xml_diff>